<commit_message>
new tables, and hr map
</commit_message>
<xml_diff>
--- a/tables/RGM EnvSx.xlsx
+++ b/tables/RGM EnvSx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewpierson/Desktop/Heloderma Spatial/Heloderma Spatial/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDD26E-3D39-1743-8E71-34A6873AC615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE84A56-A857-A74E-8A81-B1203FEA605C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="800" windowWidth="24700" windowHeight="11560" xr2:uid="{DB427BCB-D21C-CB48-B2D9-6394BCDE6647}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="57">
   <si>
     <t>Environment</t>
   </si>
@@ -340,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -478,11 +478,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,15 +576,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -588,9 +588,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CD31DA-A871-D840-AB65-4FB27201EAED}">
   <dimension ref="A3:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="92" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:P29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="92" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,24 +967,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:16" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="J3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -953,16 +996,16 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40" t="s">
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
       <c r="P4" s="35" t="s">
         <v>29</v>
       </c>
@@ -1384,239 +1427,224 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="10:16" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J20" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
+    <row r="20" spans="10:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
     </row>
     <row r="21" spans="10:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="40" t="s">
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="35" t="s">
-        <v>29</v>
-      </c>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="48"/>
     </row>
     <row r="22" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="21" t="s">
+      <c r="M22" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="N22" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P22" s="34" t="s">
-        <v>42</v>
-      </c>
+      <c r="P22" s="48"/>
     </row>
     <row r="23" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="2">
         <v>8</v>
       </c>
-      <c r="L23" s="22" t="s">
+      <c r="L23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="2">
         <v>15</v>
       </c>
-      <c r="O23" s="24" t="s">
+      <c r="O23" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="P23" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="P23" s="41"/>
     </row>
     <row r="24" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="2">
         <v>6</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="N24" s="23">
+      <c r="N24" s="53">
         <v>38</v>
       </c>
-      <c r="O24" s="22" t="s">
+      <c r="O24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="19" t="s">
-        <v>55</v>
-      </c>
+      <c r="P24" s="41"/>
     </row>
     <row r="25" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J25" s="16"/>
-      <c r="K25" s="26" t="s">
+      <c r="J25" s="54"/>
+      <c r="K25" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="23" t="s">
+      <c r="L25" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="M25" s="25"/>
-      <c r="N25" s="26" t="s">
+      <c r="M25" s="56"/>
+      <c r="N25" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="O25" s="22" t="s">
+      <c r="O25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P25" s="19"/>
+      <c r="P25" s="41"/>
     </row>
     <row r="26" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
       <c r="L26" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M26" s="29"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="31" t="s">
+      <c r="M26" s="58"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="P26" s="25"/>
+      <c r="P26" s="38"/>
     </row>
     <row r="27" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J27" s="17" t="s">
+      <c r="J27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="2">
         <v>14</v>
       </c>
-      <c r="L27" s="22" t="s">
+      <c r="L27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M27" s="19" t="s">
+      <c r="M27" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="N27" s="22">
+      <c r="N27" s="2">
         <v>15</v>
       </c>
-      <c r="O27" s="32" t="s">
+      <c r="O27" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="P27" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="P27" s="41"/>
     </row>
     <row r="28" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="2">
         <v>11</v>
       </c>
-      <c r="L28" s="22" t="s">
+      <c r="L28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="19" t="s">
+      <c r="M28" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="N28" s="23">
+      <c r="N28" s="53">
         <v>38</v>
       </c>
-      <c r="O28" s="22" t="s">
+      <c r="O28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P28" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="P28" s="41"/>
     </row>
     <row r="29" spans="10:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="47"/>
-      <c r="K29" s="36" t="s">
+      <c r="J29" s="60"/>
+      <c r="K29" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="L29" s="37" t="s">
+      <c r="L29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="M29" s="48"/>
-      <c r="N29" s="36" t="s">
+      <c r="M29" s="62"/>
+      <c r="N29" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="37" t="s">
+      <c r="O29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="P29" s="49"/>
+      <c r="P29" s="41"/>
     </row>
     <row r="30" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="41"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="38"/>
     </row>
     <row r="31" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J31" s="44"/>
+      <c r="J31" s="41"/>
       <c r="K31" s="23"/>
       <c r="L31" s="23"/>
-      <c r="M31" s="44"/>
+      <c r="M31" s="41"/>
       <c r="N31" s="23"/>
       <c r="O31" s="23"/>
       <c r="P31" s="23"/>
     </row>
     <row r="32" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J32" s="44"/>
+      <c r="J32" s="41"/>
       <c r="K32" s="23"/>
       <c r="L32" s="23"/>
-      <c r="M32" s="44"/>
+      <c r="M32" s="41"/>
       <c r="N32" s="23"/>
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
     </row>
     <row r="33" spans="10:16" x14ac:dyDescent="0.2">
-      <c r="J33" s="45"/>
-      <c r="K33" s="43"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="40"/>
       <c r="L33" s="23"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="43"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="40"/>
       <c r="O33" s="23"/>
-      <c r="P33" s="46"/>
+      <c r="P33" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="J20:P20"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="M21:O21"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J20:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>